<commit_message>
Change account number in pass-on mapping
</commit_message>
<xml_diff>
--- a/mapping/mapping_pass_on.xlsx
+++ b/mapping/mapping_pass_on.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\FO Bildrift\60 Analyse\Kontering\kontering_NN\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B30379-492A-49B5-BF6F-AF82F221085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6626A1-15B6-40E6-9C4F-47509FE12948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,10 +2443,10 @@
         <v>89</v>
       </c>
       <c r="C62" s="3">
-        <v>431200</v>
+        <v>431500</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E62" s="3">
         <v>1165</v>

</xml_diff>

<commit_message>
add method to check for missing picd in mapping_pass_on
</commit_message>
<xml_diff>
--- a/mapping/mapping_pass_on.xlsx
+++ b/mapping/mapping_pass_on.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\FO Bildrift\60 Analyse\Kontering\kontering_NN\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6626A1-15B6-40E6-9C4F-47509FE12948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E779E3F-5087-48BF-908F-F90FFF9C3C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$G$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$G$63</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="90">
   <si>
     <t>picd</t>
   </si>
@@ -702,8 +702,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204DC038-1FE0-4408-84BC-DC17332C4052}" name="Table1" displayName="Table1" ref="A1:G62" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:G62" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204DC038-1FE0-4408-84BC-DC17332C4052}" name="Table1" displayName="Table1" ref="A1:G63" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:G63" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G59">
     <sortCondition ref="A1:A59"/>
   </sortState>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,6 +2458,29 @@
         <v>73</v>
       </c>
     </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>604</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" s="3">
+        <v>431100</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1160</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change readme, gitignore and mapping
</commit_message>
<xml_diff>
--- a/mapping/mapping_pass_on.xlsx
+++ b/mapping/mapping_pass_on.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\FO Bildrift\60 Analyse\Kontering\kontering_NN\mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\Felles\Kontering LP\bildrift_lp_posting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E779E3F-5087-48BF-908F-F90FFF9C3C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A28C3C-B1A4-4B1D-BE3A-3095BE924E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
+    <workbookView xWindow="1920" yWindow="585" windowWidth="29385" windowHeight="15615" xr2:uid="{35E3EEE7-81AB-4F9F-A1FA-E066455E46C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$G$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$G$64</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="91">
   <si>
     <t>picd</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Depositum for mva tilbakeføring</t>
+  </si>
+  <si>
+    <t>El lading</t>
   </si>
 </sst>
 </file>
@@ -702,10 +705,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204DC038-1FE0-4408-84BC-DC17332C4052}" name="Table1" displayName="Table1" ref="A1:G63" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A1:G63" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G59">
-    <sortCondition ref="A1:A59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{204DC038-1FE0-4408-84BC-DC17332C4052}" name="Table1" displayName="Table1" ref="A1:G64" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:G64" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G64">
+    <sortCondition ref="A1:A64"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{8A4604BB-C61C-44BB-B659-562DB4A99C56}" name="picd" dataDxfId="6"/>
@@ -1017,22 +1020,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E92AD64-3D63-42B0-A216-0C66E47A999B}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1055,35 +1058,35 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="3">
+        <v>431500</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>100</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="3">
-        <v>431300</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1193</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>170</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="C3" s="3">
         <v>431300</v>
@@ -1101,12 +1104,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3">
         <v>431300</v>
@@ -1124,840 +1127,840 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
+        <v>199</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>431300</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1193</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>490</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="C6" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3">
         <v>1208</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>491</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="C7" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>492</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="C8" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>540</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="C9" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>541</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="C10" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>542</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="C11" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>543</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>544</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="C13" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>546</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="C14" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>548</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="C15" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>549</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="C16" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>550</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C17" s="3">
         <v>431500</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E17" s="3">
         <v>1201</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>551</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>552</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="C19" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>553</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="C20" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>554</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="C21" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>556</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="C22" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>557</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="C23" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
         <v>558</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="C24" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
         <v>562</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="C25" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>563</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C26" s="6">
         <v>431400</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E26" s="6">
         <v>1192</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>565</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C27" s="6">
         <v>431400</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E27" s="6">
         <v>1192</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>568</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C28" s="3">
         <v>420100</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E28" s="3">
         <v>1163</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>569</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C29" s="3">
         <v>420100</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E29" s="3">
         <v>1163</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>570</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="C30" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>571</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="C31" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>584</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="C32" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
         <v>586</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C33" s="6">
         <v>431400</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E33" s="6">
         <v>1192</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
         <v>587</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C34" s="6">
         <v>431400</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E34" s="6">
         <v>1192</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>591</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="C35" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="3">
         <v>1191</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="F35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>594</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="C36" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>596</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C37" s="3">
         <v>431300</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E37" s="3">
         <v>1193</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>597</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="C38" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>598</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="C39" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>603</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C40" s="3">
         <v>431100</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E40" s="3">
         <v>1160</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>607</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="3">
-        <v>431100</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1160</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>611</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>612</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C41" s="3">
         <v>431100</v>
@@ -1975,225 +1978,225 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
+        <v>607</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="3">
+        <v>431100</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1160</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>611</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>612</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>613</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="3">
+        <v>431100</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1160</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>618</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="3">
+        <v>431100</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1160</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
         <v>620</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C47" s="3">
         <v>421100</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E47" s="3">
         <v>1175</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
         <v>650</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C48" s="3">
         <v>431500</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E48" s="3">
         <v>1209</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>652</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C49" s="3">
         <v>431500</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E49" s="3">
         <v>1209</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>660</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="3">
+      <c r="C50" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="3">
         <v>1163</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
         <v>661</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="3">
-        <v>1163</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>662</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="3">
-        <v>1163</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>663</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="3">
-        <v>1163</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>667</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E49" s="3">
-        <v>1163</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>670</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="3">
-        <v>421100</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1175</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>681</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C51" s="3">
-        <v>420100</v>
+        <v>431200</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3">
         <v>1163</v>
@@ -2205,12 +2208,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>682</v>
+        <v>662</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C52" s="3">
         <v>431200</v>
@@ -2219,27 +2222,27 @@
         <v>59</v>
       </c>
       <c r="E52" s="3">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <v>690</v>
+        <v>663</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C53" s="3">
-        <v>420100</v>
+        <v>431200</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E53" s="3">
         <v>1163</v>
@@ -2251,18 +2254,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>691</v>
+        <v>667</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C54" s="3">
-        <v>420100</v>
+        <v>431200</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E54" s="3">
         <v>1163</v>
@@ -2274,211 +2277,234 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>670</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="3">
+        <v>421100</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1175</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>681</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" s="3">
+        <v>420100</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1163</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>682</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>690</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="3">
+        <v>420100</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1163</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>691</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="3">
+        <v>420100</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1163</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
         <v>792</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C60" s="6">
         <v>431400</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E60" s="6">
         <v>1192</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F60" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="G60" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
         <v>796</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C61" s="3">
         <v>431300</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E61" s="3">
         <v>1193</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
         <v>798</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C62" s="6">
         <v>431400</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E62" s="6">
         <v>1192</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F62" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G62" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
         <v>953</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C63" s="3">
         <v>421100</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E63" s="3">
         <v>1175</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
         <v>958</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E59" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>543</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E60" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>551</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="3">
-        <v>431200</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>37</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="3">
-        <v>431500</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E62" s="3">
-        <v>1165</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>604</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" s="3">
-        <v>431100</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E63" s="3">
-        <v>1160</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>71</v>
+      <c r="C64" s="3">
+        <v>431200</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1165</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>